<commit_message>
Fixed the logic for the loop when inputting values into the excel file. Iterating through a dict of dicts, everything seems to work correctly except some small values that don't add up to what the net columns say in the actual downloaded csv file.
</commit_message>
<xml_diff>
--- a/WSIG DCF Output.xlsx
+++ b/WSIG DCF Output.xlsx
@@ -457,9 +457,9 @@
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="43"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164"/>
   </cellStyleXfs>
   <cellXfs count="123">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -768,7 +768,7 @@
     <cellStyle builtinId="5" name="Percent" xfId="2"/>
     <cellStyle builtinId="4" name="Currency" xfId="3"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -780,193 +780,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -2722,11 +2535,21 @@
       <c r="A15" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="94" t="n"/>
-      <c r="C15" s="94" t="n"/>
-      <c r="D15" s="94" t="n"/>
-      <c r="E15" s="94" t="n"/>
-      <c r="F15" s="94" t="n"/>
+      <c r="B15" s="94" t="n">
+        <v>11257</v>
+      </c>
+      <c r="C15" s="94" t="n">
+        <v>11636</v>
+      </c>
+      <c r="D15" s="94" t="n">
+        <v>11634</v>
+      </c>
+      <c r="E15" s="94" t="n">
+        <v>11076</v>
+      </c>
+      <c r="F15" s="94" t="n">
+        <v>10505</v>
+      </c>
       <c r="G15" s="100" t="n"/>
       <c r="H15" s="101">
         <f>H4*Assumptions!B23</f>
@@ -2763,11 +2586,21 @@
       <c r="A16" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="94" t="n"/>
-      <c r="C16" s="94" t="n"/>
-      <c r="D16" s="94" t="n"/>
-      <c r="E16" s="94" t="n"/>
-      <c r="F16" s="94" t="n"/>
+      <c r="B16" s="94" t="n">
+        <v>-11488</v>
+      </c>
+      <c r="C16" s="94" t="n">
+        <v>-12229</v>
+      </c>
+      <c r="D16" s="94" t="n">
+        <v>-12352</v>
+      </c>
+      <c r="E16" s="94" t="n">
+        <v>-13168</v>
+      </c>
+      <c r="F16" s="94" t="n">
+        <v>-13548</v>
+      </c>
       <c r="G16" s="100" t="n"/>
       <c r="H16" s="101">
         <f>Assumptions!B24*'Base Case'!H4</f>
@@ -2880,11 +2713,21 @@
       <c r="A19" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="94" t="n"/>
-      <c r="C19" s="94" t="n"/>
-      <c r="D19" s="94" t="n"/>
-      <c r="E19" s="94" t="n"/>
-      <c r="F19" s="94" t="n"/>
+      <c r="B19" s="94" t="n">
+        <v>791</v>
+      </c>
+      <c r="C19" s="94" t="n">
+        <v>1764</v>
+      </c>
+      <c r="D19" s="94" t="n">
+        <v>2111</v>
+      </c>
+      <c r="E19" s="94" t="n">
+        <v>2349</v>
+      </c>
+      <c r="F19" s="94" t="n">
+        <v>2132</v>
+      </c>
       <c r="G19" s="100" t="n"/>
       <c r="H19" s="101" t="n"/>
       <c r="I19" s="101" t="n"/>
@@ -2906,11 +2749,21 @@
       <c r="A20" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="94" t="n"/>
-      <c r="C20" s="94" t="n"/>
-      <c r="D20" s="94" t="n"/>
-      <c r="E20" s="94" t="n"/>
-      <c r="F20" s="94" t="n"/>
+      <c r="B20" s="94" t="n">
+        <v>18383</v>
+      </c>
+      <c r="C20" s="94" t="n">
+        <v>26287</v>
+      </c>
+      <c r="D20" s="94" t="n">
+        <v>11233</v>
+      </c>
+      <c r="E20" s="94" t="n">
+        <v>20481</v>
+      </c>
+      <c r="F20" s="94" t="n">
+        <v>46671</v>
+      </c>
       <c r="G20" s="100" t="n"/>
       <c r="H20" s="101" t="n"/>
       <c r="I20" s="101" t="n"/>
@@ -2932,11 +2785,21 @@
       <c r="A21" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="94" t="n"/>
-      <c r="C21" s="94" t="n"/>
-      <c r="D21" s="94" t="n"/>
-      <c r="E21" s="94" t="n"/>
-      <c r="F21" s="94" t="n"/>
+      <c r="B21" s="94" t="n">
+        <v>57653</v>
+      </c>
+      <c r="C21" s="94" t="n">
+        <v>73286</v>
+      </c>
+      <c r="D21" s="94" t="n">
+        <v>68531</v>
+      </c>
+      <c r="E21" s="94" t="n">
+        <v>89378</v>
+      </c>
+      <c r="F21" s="94" t="n">
+        <v>106869</v>
+      </c>
       <c r="G21" s="100" t="n"/>
       <c r="H21" s="101" t="n"/>
       <c r="I21" s="101" t="n"/>
@@ -2958,11 +2821,21 @@
       <c r="A22" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="94" t="n"/>
-      <c r="C22" s="94" t="n"/>
-      <c r="D22" s="94" t="n"/>
-      <c r="E22" s="94" t="n"/>
-      <c r="F22" s="94" t="n"/>
+      <c r="B22" s="94" t="n">
+        <v>176064</v>
+      </c>
+      <c r="C22" s="94" t="n">
+        <v>207000</v>
+      </c>
+      <c r="D22" s="94" t="n">
+        <v>231839</v>
+      </c>
+      <c r="E22" s="94" t="n">
+        <v>290345</v>
+      </c>
+      <c r="F22" s="94" t="n">
+        <v>321686</v>
+      </c>
       <c r="G22" s="100" t="n"/>
       <c r="H22" s="101" t="n"/>
       <c r="I22" s="101" t="n"/>
@@ -2984,11 +2857,21 @@
       <c r="A23" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="94" t="n"/>
-      <c r="C23" s="94" t="n"/>
-      <c r="D23" s="94" t="n"/>
-      <c r="E23" s="94" t="n"/>
-      <c r="F23" s="94" t="n"/>
+      <c r="B23" s="94" t="n">
+        <v/>
+      </c>
+      <c r="C23" s="94" t="n">
+        <v/>
+      </c>
+      <c r="D23" s="94" t="n">
+        <v>6308</v>
+      </c>
+      <c r="E23" s="94" t="n">
+        <v>10999</v>
+      </c>
+      <c r="F23" s="94" t="n">
+        <v>11605</v>
+      </c>
       <c r="G23" s="100" t="n"/>
       <c r="H23" s="101" t="n"/>
       <c r="I23" s="101" t="n"/>
@@ -3010,11 +2893,21 @@
       <c r="A24" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="94" t="n"/>
-      <c r="C24" s="94" t="n"/>
-      <c r="D24" s="94" t="n"/>
-      <c r="E24" s="94" t="n"/>
-      <c r="F24" s="94" t="n"/>
+      <c r="B24" s="94" t="n">
+        <v>38542</v>
+      </c>
+      <c r="C24" s="94" t="n">
+        <v>43658</v>
+      </c>
+      <c r="D24" s="94" t="n">
+        <v>63448</v>
+      </c>
+      <c r="E24" s="94" t="n">
+        <v>80610</v>
+      </c>
+      <c r="F24" s="94" t="n">
+        <v>79006</v>
+      </c>
       <c r="G24" s="100" t="n"/>
       <c r="H24" s="101" t="n"/>
       <c r="I24" s="101" t="n"/>
@@ -3036,11 +2929,21 @@
       <c r="A25" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="94" t="n"/>
-      <c r="C25" s="94" t="n"/>
-      <c r="D25" s="94" t="n"/>
-      <c r="E25" s="94" t="n"/>
-      <c r="F25" s="94" t="n"/>
+      <c r="B25" s="94" t="n">
+        <v/>
+      </c>
+      <c r="C25" s="94" t="n">
+        <v>16960</v>
+      </c>
+      <c r="D25" s="94" t="n">
+        <v>28987</v>
+      </c>
+      <c r="E25" s="94" t="n">
+        <v>53329</v>
+      </c>
+      <c r="F25" s="94" t="n">
+        <v>75427</v>
+      </c>
       <c r="G25" s="100" t="n"/>
       <c r="H25" s="101" t="n"/>
       <c r="I25" s="101" t="n"/>
@@ -3062,11 +2965,21 @@
       <c r="A26" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="94" t="n"/>
-      <c r="C26" s="94" t="n"/>
-      <c r="D26" s="94" t="n"/>
-      <c r="E26" s="94" t="n"/>
-      <c r="F26" s="94" t="n"/>
+      <c r="B26" s="94" t="n">
+        <v>57854</v>
+      </c>
+      <c r="C26" s="94" t="n">
+        <v>83451</v>
+      </c>
+      <c r="D26" s="94" t="n">
+        <v>120292</v>
+      </c>
+      <c r="E26" s="94" t="n">
+        <v>170990</v>
+      </c>
+      <c r="F26" s="94" t="n">
+        <v>193437</v>
+      </c>
       <c r="G26" s="100" t="n"/>
       <c r="H26" s="101" t="n"/>
       <c r="I26" s="101" t="n"/>
@@ -3088,11 +3001,21 @@
       <c r="A27" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="94" t="n"/>
-      <c r="C27" s="94" t="n"/>
-      <c r="D27" s="94" t="n"/>
-      <c r="E27" s="94" t="n"/>
-      <c r="F27" s="94" t="n"/>
+      <c r="B27" s="94" t="n">
+        <v>118210</v>
+      </c>
+      <c r="C27" s="94" t="n">
+        <v>123549</v>
+      </c>
+      <c r="D27" s="94" t="n">
+        <v>111547</v>
+      </c>
+      <c r="E27" s="94" t="n">
+        <v>119355</v>
+      </c>
+      <c r="F27" s="94" t="n">
+        <v>128249</v>
+      </c>
       <c r="G27" s="100" t="n"/>
       <c r="H27" s="101" t="n"/>
       <c r="I27" s="101" t="n"/>
@@ -3293,32 +3216,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule dxfId="2" priority="8" type="expression">
+    <cfRule dxfId="1" priority="8" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O5">
-    <cfRule dxfId="3" priority="6" type="expression">
+    <cfRule dxfId="0" priority="6" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule dxfId="4" priority="5" type="expression">
+    <cfRule dxfId="0" priority="5" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9:O11">
-    <cfRule dxfId="5" priority="4" type="expression">
+    <cfRule dxfId="0" priority="4" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15:O16">
-    <cfRule dxfId="6" priority="3" type="expression">
+    <cfRule dxfId="0" priority="3" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O19:O27">
-    <cfRule dxfId="7" priority="1" type="expression">
+    <cfRule dxfId="0" priority="1" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4765,47 +4688,47 @@
   </sheetData>
   <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="1" pivotTables="1" scenarios="1" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
   <conditionalFormatting sqref="G4:G5">
-    <cfRule dxfId="8" priority="9" type="expression">
+    <cfRule dxfId="0" priority="9" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G11 G15:G16 G19:G27">
-    <cfRule dxfId="9" priority="8" type="expression">
+    <cfRule dxfId="1" priority="8" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule dxfId="10" priority="7" type="expression">
+    <cfRule dxfId="1" priority="7" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N5">
-    <cfRule dxfId="11" priority="6" type="expression">
+    <cfRule dxfId="0" priority="6" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O5">
-    <cfRule dxfId="12" priority="5" type="expression">
+    <cfRule dxfId="0" priority="5" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:O7">
-    <cfRule dxfId="13" priority="4" type="expression">
+    <cfRule dxfId="0" priority="4" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9:O11">
-    <cfRule dxfId="14" priority="3" type="expression">
+    <cfRule dxfId="0" priority="3" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:O16">
-    <cfRule dxfId="15" priority="2" type="expression">
+    <cfRule dxfId="0" priority="2" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19:N27">
-    <cfRule dxfId="16" priority="1" type="expression">
+    <cfRule dxfId="0" priority="1" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6251,47 +6174,47 @@
   </sheetData>
   <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="1" pivotTables="1" scenarios="1" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
   <conditionalFormatting sqref="G4:G5">
-    <cfRule dxfId="17" priority="9" type="expression">
+    <cfRule dxfId="0" priority="9" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G11 G15:G16 G19:G27">
-    <cfRule dxfId="18" priority="8" type="expression">
+    <cfRule dxfId="1" priority="8" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule dxfId="19" priority="7" type="expression">
+    <cfRule dxfId="1" priority="7" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N5">
-    <cfRule dxfId="20" priority="6" type="expression">
+    <cfRule dxfId="0" priority="6" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O5">
-    <cfRule dxfId="21" priority="5" type="expression">
+    <cfRule dxfId="0" priority="5" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:O7">
-    <cfRule dxfId="22" priority="4" type="expression">
+    <cfRule dxfId="0" priority="4" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9:O11">
-    <cfRule dxfId="23" priority="3" type="expression">
+    <cfRule dxfId="0" priority="3" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:O16">
-    <cfRule dxfId="24" priority="2" type="expression">
+    <cfRule dxfId="0" priority="2" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19:N27">
-    <cfRule dxfId="25" priority="1" type="expression">
+    <cfRule dxfId="0" priority="1" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Went through and fixed minor mistakes in the layout of the excel cell population. Re-commented a lot of sections so it is up to date with the changes that have been made. Only element that doesn't add up with SEC data is the current portion of liabilities; need to check that out still. Also added very basic safeguards for check to see if the data matches up to the sec data. Haven't tried running the safeguards, so if the code doesn't compile then its likely the suspect.
</commit_message>
<xml_diff>
--- a/WSIG DCF Output.xlsx
+++ b/WSIG DCF Output.xlsx
@@ -2174,19 +2174,19 @@
         <v>46</v>
       </c>
       <c r="B7" s="94" t="n">
-        <v>10040</v>
+        <v>13421</v>
       </c>
       <c r="C7" s="94" t="n">
-        <v>10830</v>
+        <v>15305</v>
       </c>
       <c r="D7" s="94" t="n">
-        <v>11993</v>
+        <v>18034</v>
       </c>
       <c r="E7" s="94" t="n">
-        <v>14329</v>
+        <v>22396</v>
       </c>
       <c r="F7" s="94" t="n">
-        <v>14194</v>
+        <v>24239</v>
       </c>
       <c r="G7" s="100" t="n"/>
       <c r="H7" s="101" t="n"/>
@@ -2536,19 +2536,19 @@
         <v>53</v>
       </c>
       <c r="B15" s="94" t="n">
-        <v>11257</v>
+        <v>-11488</v>
       </c>
       <c r="C15" s="94" t="n">
-        <v>11636</v>
+        <v>-12229</v>
       </c>
       <c r="D15" s="94" t="n">
-        <v>11634</v>
+        <v>-12352</v>
       </c>
       <c r="E15" s="94" t="n">
-        <v>11076</v>
+        <v>-13168</v>
       </c>
       <c r="F15" s="94" t="n">
-        <v>10505</v>
+        <v>-13548</v>
       </c>
       <c r="G15" s="100" t="n"/>
       <c r="H15" s="101">
@@ -2587,19 +2587,19 @@
         <v>54</v>
       </c>
       <c r="B16" s="94" t="n">
-        <v>-11488</v>
+        <v>11257</v>
       </c>
       <c r="C16" s="94" t="n">
-        <v>-12229</v>
+        <v>11636</v>
       </c>
       <c r="D16" s="94" t="n">
-        <v>-12352</v>
+        <v>11634</v>
       </c>
       <c r="E16" s="94" t="n">
-        <v>-13168</v>
+        <v>11076</v>
       </c>
       <c r="F16" s="94" t="n">
-        <v>-13548</v>
+        <v>10505</v>
       </c>
       <c r="G16" s="100" t="n"/>
       <c r="H16" s="101">

</xml_diff>

<commit_message>
Changes to readme and fixed the initial QA implementations for the Income Statement. Really need to focus on dealing with the different naming conventions.
</commit_message>
<xml_diff>
--- a/WSIG DCF Output.xlsx
+++ b/WSIG DCF Output.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
   <si>
     <t xml:space="preserve">WHITWORTH STUDENT INVESTMENT GROUP </t>
   </si>
@@ -32,6 +32,9 @@
     <t>Stock Symbol</t>
   </si>
   <si>
+    <t>AAPL</t>
+  </si>
+  <si>
     <t>Sector</t>
   </si>
   <si>
@@ -47,7 +50,13 @@
     <t>Period Ending Date of Last 10Q</t>
   </si>
   <si>
+    <t>9/18/2016</t>
+  </si>
+  <si>
     <t>Period Ending Date of Last 10K</t>
+  </si>
+  <si>
+    <t>12/18/2016</t>
   </si>
   <si>
     <t>DCF Last Updated</t>
@@ -457,9 +466,9 @@
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="43"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="123">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -768,7 +777,7 @@
     <cellStyle builtinId="5" name="Percent" xfId="2"/>
     <cellStyle builtinId="4" name="Currency" xfId="3"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="26">
     <dxf>
       <fill>
         <patternFill>
@@ -780,6 +789,193 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -1242,47 +1438,53 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="78" t="n"/>
+      <c r="B4" s="78" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="78" t="n"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="78" t="n"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="78" t="n"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="79" t="n"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="79" t="n"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="79" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="79" t="n"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="79" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" s="79" t="n"/>
     </row>
@@ -1314,7 +1516,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="22" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1322,7 +1524,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="3" s="21" spans="1:9" thickBot="1">
       <c r="A3" s="25" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="58">
         <f>'Base Case'!B3</f>
@@ -1349,15 +1551,15 @@
         <v/>
       </c>
       <c r="I3" s="58" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="27" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="91" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" s="92">
         <f>IF(OR(ISERROR('Base Case'!C4/'Base Case'!B4),'Base Case'!B4&lt;0,'Base Case'!C4&lt;0),"NA",'Base Case'!C4/'Base Case'!B4-1)</f>
@@ -1376,7 +1578,7 @@
         <v/>
       </c>
       <c r="G4" s="92" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I4" s="92">
         <f>IF(ISERROR(AVERAGE(B4:F4)),"NA",AVERAGE(B4:F4))</f>
@@ -1385,7 +1587,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="27" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="92">
         <f>IF(ISERROR('Base Case'!B8/'Base Case'!B4),"NA",'Base Case'!B8/'Base Case'!B4)</f>
@@ -1418,7 +1620,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="27" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B6" s="92">
         <f>IF(ISERROR('Base Case'!B10/'Base Case'!B9),"NA",'Base Case'!B10/'Base Case'!B9)</f>
@@ -1451,7 +1653,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="27" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B7" s="92">
         <f>IF(ISERROR('Base Case'!B16/'Base Case'!B4),"NA",'Base Case'!B16/'Base Case'!B4)</f>
@@ -1484,7 +1686,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="27" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B8" s="92">
         <f>IF(ISERROR('Base Case'!B15/'Base Case'!B4),"NA",'Base Case'!B15/'Base Case'!B4)</f>
@@ -1517,7 +1719,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="27" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B9" s="92">
         <f>IF(ISERROR('Base Case'!B29/'Base Case'!B4),"NA",'Base Case'!B29/'Base Case'!B4)</f>
@@ -1559,7 +1761,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="11" s="21" spans="1:9" thickBot="1">
       <c r="A11" s="25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B11" s="93" t="n"/>
       <c r="C11" s="93" t="n"/>
@@ -1571,11 +1773,11 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="27" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B12" s="94" t="n"/>
       <c r="D12" s="95" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F12" s="83" t="n"/>
       <c r="G12" s="92" t="n"/>
@@ -1583,11 +1785,11 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="27" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B13" s="96" t="n"/>
       <c r="D13" s="95" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F13" s="97" t="n"/>
       <c r="G13" s="92" t="n"/>
@@ -1595,11 +1797,11 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="27" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="96" t="n"/>
       <c r="D14" s="95" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F14" s="85" t="n"/>
       <c r="G14" s="92" t="n"/>
@@ -1607,11 +1809,11 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="27" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B15" s="96" t="n"/>
       <c r="D15" s="95" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F15" s="83" t="n"/>
       <c r="G15" s="92" t="n"/>
@@ -1619,11 +1821,11 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="27" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B16" s="96" t="n"/>
       <c r="D16" s="95" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F16" s="94" t="n"/>
       <c r="G16" s="92" t="n"/>
@@ -1631,11 +1833,11 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="27" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B17" s="96" t="n"/>
       <c r="D17" s="95" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F17" s="83" t="n"/>
       <c r="G17" s="92" t="n"/>
@@ -1643,7 +1845,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="19" s="21" spans="1:9" thickBot="1">
       <c r="A19" s="25" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B19" s="58">
         <f>'Base Case'!H3</f>
@@ -1668,7 +1870,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="27" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B20" s="98" t="n"/>
       <c r="C20" s="98" t="n"/>
@@ -1678,7 +1880,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="27" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B21" s="98" t="n"/>
       <c r="C21" s="98" t="n"/>
@@ -1688,7 +1890,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="27" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B22" s="98" t="n"/>
       <c r="C22" s="98" t="n"/>
@@ -1698,7 +1900,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="27" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B23" s="98" t="n"/>
       <c r="C23" s="98" t="n"/>
@@ -1708,7 +1910,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="27" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B24" s="98" t="n"/>
       <c r="C24" s="98" t="n"/>
@@ -1721,7 +1923,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="27" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B25" s="98" t="n"/>
       <c r="C25" s="98" t="n"/>
@@ -1731,13 +1933,13 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B26" s="98" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="28" s="21" spans="1:9" thickBot="1">
       <c r="A28" s="25" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B28" s="58">
         <f>B19</f>
@@ -1762,7 +1964,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="27" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B29" s="98" t="n"/>
       <c r="C29" s="98" t="n"/>
@@ -1772,7 +1974,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="27" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B30" s="98" t="n"/>
       <c r="C30" s="98" t="n"/>
@@ -1782,7 +1984,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="27" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B31" s="98" t="n"/>
       <c r="C31" s="98" t="n"/>
@@ -1792,7 +1994,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="27" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B32" s="98" t="n"/>
       <c r="C32" s="98" t="n"/>
@@ -1802,7 +2004,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="27" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B33" s="98" t="n"/>
       <c r="C33" s="98" t="n"/>
@@ -1815,7 +2017,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="27" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B34" s="98" t="n"/>
       <c r="C34" s="98" t="n"/>
@@ -1825,13 +2027,13 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B35" s="98" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="37" s="21" spans="1:9" thickBot="1">
       <c r="A37" s="25" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B37" s="58">
         <f>B19</f>
@@ -1856,7 +2058,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="27" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B38" s="98" t="n"/>
       <c r="C38" s="98" t="n"/>
@@ -1866,7 +2068,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="27" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B39" s="98" t="n"/>
       <c r="C39" s="98" t="n"/>
@@ -1876,7 +2078,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="27" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B40" s="98" t="n"/>
       <c r="C40" s="98" t="n"/>
@@ -1886,7 +2088,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="27" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B41" s="98" t="n"/>
       <c r="C41" s="98" t="n"/>
@@ -1896,7 +2098,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="27" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B42" s="98" t="n"/>
       <c r="C42" s="98" t="n"/>
@@ -1909,7 +2111,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="27" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B43" s="98" t="n"/>
       <c r="C43" s="98" t="n"/>
@@ -1919,7 +2121,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B44" s="98" t="n"/>
     </row>
@@ -1954,12 +2156,12 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="B2" s="45" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C2" s="45" t="n"/>
       <c r="D2" s="45" t="n"/>
@@ -1967,7 +2169,7 @@
       <c r="F2" s="45" t="n"/>
       <c r="G2" s="45" t="n"/>
       <c r="H2" s="45" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I2" s="45" t="n"/>
       <c r="J2" s="45" t="n"/>
@@ -1976,7 +2178,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="3" s="21" spans="1:17" thickBot="1">
       <c r="A3" s="25" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="58">
         <f>YEAR('Title Page'!B11)-4</f>
@@ -2032,12 +2234,12 @@
         <v/>
       </c>
       <c r="P3" s="58" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="27" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B4" s="94" t="n">
         <v>156508</v>
@@ -2088,7 +2290,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="27" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B5" s="94" t="n">
         <v>87846</v>
@@ -2124,7 +2326,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="76" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B6" s="103">
         <f>B4-B5</f>
@@ -2171,7 +2373,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B7" s="94" t="n">
         <v>13421</v>
@@ -2207,7 +2409,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="76" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B8" s="103">
         <f>B6-B7</f>
@@ -2269,7 +2471,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="27" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B9" s="94" t="n">
         <v>55763</v>
@@ -2320,7 +2522,7 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B10" s="94" t="n">
         <v>14030</v>
@@ -2371,7 +2573,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="27" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B11" s="94" t="n">
         <v>522</v>
@@ -2407,7 +2609,7 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="76" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B12" s="103">
         <f>B9-B10+B11</f>
@@ -2471,7 +2673,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="14" s="21" spans="1:17" thickBot="1">
       <c r="A14" s="25" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B14" s="58">
         <f>B3</f>
@@ -2533,7 +2735,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="27" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B15" s="94" t="n">
         <v>-11488</v>
@@ -2584,7 +2786,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="27" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B16" s="94" t="n">
         <v>11257</v>
@@ -2652,7 +2854,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="18" s="21" spans="1:17" thickBot="1">
       <c r="A18" s="25" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B18" s="58">
         <f>B14</f>
@@ -2711,7 +2913,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="27" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B19" s="94" t="n">
         <v>791</v>
@@ -2747,22 +2949,22 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="27" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B20" s="94" t="n">
-        <v>18383</v>
+        <v>29129</v>
       </c>
       <c r="C20" s="94" t="n">
-        <v>26287</v>
+        <v>40546</v>
       </c>
       <c r="D20" s="94" t="n">
-        <v>11233</v>
+        <v>25077</v>
       </c>
       <c r="E20" s="94" t="n">
-        <v>20481</v>
+        <v>41601</v>
       </c>
       <c r="F20" s="94" t="n">
-        <v>46671</v>
+        <v>67155</v>
       </c>
       <c r="G20" s="100" t="n"/>
       <c r="H20" s="101" t="n"/>
@@ -2783,7 +2985,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="27" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B21" s="94" t="n">
         <v>57653</v>
@@ -2819,7 +3021,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="27" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B22" s="94" t="n">
         <v>176064</v>
@@ -2855,7 +3057,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="27" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B23" s="94" t="n">
         <v/>
@@ -2891,7 +3093,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="27" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B24" s="94" t="n">
         <v>38542</v>
@@ -2927,7 +3129,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="27" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B25" s="94" t="n">
         <v/>
@@ -2963,7 +3165,7 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="27" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B26" s="94" t="n">
         <v>57854</v>
@@ -2999,7 +3201,7 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="27" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B27" s="94" t="n">
         <v>118210</v>
@@ -3035,7 +3237,7 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="17" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B28" s="101">
         <f>B22-B26-B27</f>
@@ -3093,7 +3295,7 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="29" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B29" s="103">
         <f>B21-B24-B20+B23</f>
@@ -3152,7 +3354,7 @@
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="29" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B30" s="106" t="n"/>
       <c r="C30" s="107">
@@ -3216,32 +3418,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule dxfId="1" priority="8" type="expression">
+    <cfRule dxfId="2" priority="8" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O5">
-    <cfRule dxfId="0" priority="6" type="expression">
+    <cfRule dxfId="3" priority="6" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule dxfId="0" priority="5" type="expression">
+    <cfRule dxfId="4" priority="5" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9:O11">
-    <cfRule dxfId="0" priority="4" type="expression">
+    <cfRule dxfId="5" priority="4" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15:O16">
-    <cfRule dxfId="0" priority="3" type="expression">
+    <cfRule dxfId="6" priority="3" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O19:O27">
-    <cfRule dxfId="0" priority="1" type="expression">
+    <cfRule dxfId="7" priority="1" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3275,12 +3477,12 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="B2" s="45" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C2" s="45" t="n"/>
       <c r="D2" s="45" t="n"/>
@@ -3288,7 +3490,7 @@
       <c r="F2" s="45" t="n"/>
       <c r="G2" s="45" t="n"/>
       <c r="H2" s="45" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I2" s="45" t="n"/>
       <c r="J2" s="45" t="n"/>
@@ -3297,7 +3499,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="3" s="21" spans="1:17" thickBot="1">
       <c r="A3" s="25" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="58">
         <f>YEAR('Title Page'!B11)-4</f>
@@ -3353,12 +3555,12 @@
         <v/>
       </c>
       <c r="P3" s="58" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="27" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B4" s="109">
         <f>'Base Case'!B4</f>
@@ -3420,7 +3622,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="27" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B5" s="109">
         <f>'Base Case'!B5</f>
@@ -3467,7 +3669,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="76" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B6" s="103">
         <f>B4-B5</f>
@@ -3514,7 +3716,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B7" s="109">
         <f>'Base Case'!B7</f>
@@ -3561,7 +3763,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="76" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B8" s="103">
         <f>B6-B7</f>
@@ -3623,7 +3825,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="27" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B9" s="109">
         <f>'Base Case'!B9</f>
@@ -3685,7 +3887,7 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B10" s="109">
         <f>'Base Case'!B10</f>
@@ -3747,7 +3949,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="27" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B11" s="109">
         <f>'Base Case'!B11</f>
@@ -3794,7 +3996,7 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="76" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B12" s="103">
         <f>B9-B10-B11</f>
@@ -3858,7 +4060,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="14" s="21" spans="1:17" thickBot="1">
       <c r="A14" s="25" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B14" s="58">
         <f>B3</f>
@@ -3920,7 +4122,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="27" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B15" s="109">
         <f>'Base Case'!B15</f>
@@ -3982,7 +4184,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="27" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B16" s="109">
         <f>'Base Case'!B16</f>
@@ -4061,7 +4263,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="18" s="21" spans="1:17" thickBot="1">
       <c r="A18" s="25" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B18" s="58">
         <f>B14</f>
@@ -4120,7 +4322,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="27" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B19" s="109">
         <f>'Base Case'!B19</f>
@@ -4164,7 +4366,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="27" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B20" s="109">
         <f>'Base Case'!B20</f>
@@ -4208,7 +4410,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="27" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B21" s="109">
         <f>'Base Case'!B21</f>
@@ -4252,7 +4454,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="27" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B22" s="109">
         <f>'Base Case'!B22</f>
@@ -4296,7 +4498,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="27" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B23" s="109">
         <f>'Base Case'!B23</f>
@@ -4340,7 +4542,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="27" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B24" s="109">
         <f>'Base Case'!B24</f>
@@ -4384,7 +4586,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="27" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B25" s="109">
         <f>'Base Case'!B25</f>
@@ -4425,7 +4627,7 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="27" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B26" s="109">
         <f>'Base Case'!B26</f>
@@ -4469,7 +4671,7 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="27" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B27" s="109">
         <f>'Base Case'!B27</f>
@@ -4513,7 +4715,7 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="17" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B28" s="101">
         <f>B22-B26-B27</f>
@@ -4572,7 +4774,7 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="29" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B29" s="103">
         <f>B21-B24-B20+B23</f>
@@ -4631,7 +4833,7 @@
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="29" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B30" s="107">
         <f>'Base Case'!B30</f>
@@ -4688,47 +4890,47 @@
   </sheetData>
   <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="1" pivotTables="1" scenarios="1" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
   <conditionalFormatting sqref="G4:G5">
-    <cfRule dxfId="0" priority="9" type="expression">
+    <cfRule dxfId="8" priority="9" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G11 G15:G16 G19:G27">
-    <cfRule dxfId="1" priority="8" type="expression">
+    <cfRule dxfId="9" priority="8" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule dxfId="1" priority="7" type="expression">
+    <cfRule dxfId="10" priority="7" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N5">
-    <cfRule dxfId="0" priority="6" type="expression">
+    <cfRule dxfId="11" priority="6" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O5">
-    <cfRule dxfId="0" priority="5" type="expression">
+    <cfRule dxfId="12" priority="5" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:O7">
-    <cfRule dxfId="0" priority="4" type="expression">
+    <cfRule dxfId="13" priority="4" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9:O11">
-    <cfRule dxfId="0" priority="3" type="expression">
+    <cfRule dxfId="14" priority="3" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:O16">
-    <cfRule dxfId="0" priority="2" type="expression">
+    <cfRule dxfId="15" priority="2" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19:N27">
-    <cfRule dxfId="0" priority="1" type="expression">
+    <cfRule dxfId="16" priority="1" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4761,12 +4963,12 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="B2" s="45" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C2" s="45" t="n"/>
       <c r="D2" s="45" t="n"/>
@@ -4774,7 +4976,7 @@
       <c r="F2" s="45" t="n"/>
       <c r="G2" s="45" t="n"/>
       <c r="H2" s="45" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I2" s="45" t="n"/>
       <c r="J2" s="45" t="n"/>
@@ -4783,7 +4985,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="3" s="21" spans="1:17" thickBot="1">
       <c r="A3" s="25" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" s="58">
         <f>YEAR('Title Page'!B11)-4</f>
@@ -4839,12 +5041,12 @@
         <v/>
       </c>
       <c r="P3" s="58" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="27" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B4" s="109">
         <f>'Base Case'!B4</f>
@@ -4906,7 +5108,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="27" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B5" s="109">
         <f>'Base Case'!B5</f>
@@ -4953,7 +5155,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="76" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B6" s="103">
         <f>B4-B5</f>
@@ -5000,7 +5202,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B7" s="109">
         <f>'Base Case'!B7</f>
@@ -5047,7 +5249,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="76" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B8" s="103">
         <f>B6-B7</f>
@@ -5109,7 +5311,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="27" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B9" s="109">
         <f>'Base Case'!B9</f>
@@ -5171,7 +5373,7 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="16" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B10" s="109">
         <f>'Base Case'!B10</f>
@@ -5233,7 +5435,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="27" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B11" s="109">
         <f>'Base Case'!B11</f>
@@ -5280,7 +5482,7 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="76" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B12" s="103">
         <f>B9-B10-B11</f>
@@ -5344,7 +5546,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="14" s="21" spans="1:17" thickBot="1">
       <c r="A14" s="25" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B14" s="58">
         <f>B3</f>
@@ -5406,7 +5608,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="27" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B15" s="109">
         <f>'Base Case'!B15</f>
@@ -5468,7 +5670,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="27" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B16" s="109">
         <f>'Base Case'!B16</f>
@@ -5547,7 +5749,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="18" s="21" spans="1:17" thickBot="1">
       <c r="A18" s="25" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B18" s="58">
         <f>B14</f>
@@ -5606,7 +5808,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="27" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B19" s="109">
         <f>'Base Case'!B19</f>
@@ -5650,7 +5852,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="27" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B20" s="109">
         <f>'Base Case'!B20</f>
@@ -5694,7 +5896,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="27" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B21" s="109">
         <f>'Base Case'!B21</f>
@@ -5738,7 +5940,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="27" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B22" s="109">
         <f>'Base Case'!B22</f>
@@ -5782,7 +5984,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="27" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B23" s="109">
         <f>'Base Case'!B23</f>
@@ -5826,7 +6028,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="27" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B24" s="109">
         <f>'Base Case'!B24</f>
@@ -5870,7 +6072,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="27" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B25" s="109">
         <f>'Base Case'!B25</f>
@@ -5911,7 +6113,7 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="27" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B26" s="109">
         <f>'Base Case'!B26</f>
@@ -5955,7 +6157,7 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="27" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B27" s="109">
         <f>'Base Case'!B27</f>
@@ -5999,7 +6201,7 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="17" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B28" s="101">
         <f>B22-B26-B27</f>
@@ -6058,7 +6260,7 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="29" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B29" s="103">
         <f>B21-B24-B20+B23</f>
@@ -6117,7 +6319,7 @@
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="29" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B30" s="107">
         <f>'Base Case'!B30</f>
@@ -6174,47 +6376,47 @@
   </sheetData>
   <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="1" pivotTables="1" scenarios="1" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
   <conditionalFormatting sqref="G4:G5">
-    <cfRule dxfId="0" priority="9" type="expression">
+    <cfRule dxfId="17" priority="9" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G11 G15:G16 G19:G27">
-    <cfRule dxfId="1" priority="8" type="expression">
+    <cfRule dxfId="18" priority="8" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule dxfId="1" priority="7" type="expression">
+    <cfRule dxfId="19" priority="7" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N5">
-    <cfRule dxfId="0" priority="6" type="expression">
+    <cfRule dxfId="20" priority="6" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O5">
-    <cfRule dxfId="0" priority="5" type="expression">
+    <cfRule dxfId="21" priority="5" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:O7">
-    <cfRule dxfId="0" priority="4" type="expression">
+    <cfRule dxfId="22" priority="4" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9:O11">
-    <cfRule dxfId="0" priority="3" type="expression">
+    <cfRule dxfId="23" priority="3" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:O16">
-    <cfRule dxfId="0" priority="2" type="expression">
+    <cfRule dxfId="24" priority="2" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19:N27">
-    <cfRule dxfId="0" priority="1" type="expression">
+    <cfRule dxfId="25" priority="1" type="expression">
       <formula>$G$3="NA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6243,17 +6445,17 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="22" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="22" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B4" s="6">
         <f>Assumptions!$F$12</f>
@@ -6262,7 +6464,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B5" s="28">
         <f>Assumptions!$F$17</f>
@@ -6271,7 +6473,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2">
         <f>Assumptions!$F$13</f>
@@ -6280,7 +6482,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B7" s="6">
         <f>B4+(B6*(B5-B4))</f>
@@ -6289,12 +6491,12 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="22" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <f>Assumptions!$F$14</f>
@@ -6303,7 +6505,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B11" s="6">
         <f>Assumptions!$F$15</f>
@@ -6312,7 +6514,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B12" s="6">
         <f>MAX(B10:B11)</f>
@@ -6321,7 +6523,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B13" s="7">
         <f>Assumptions!$G$6</f>
@@ -6330,7 +6532,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B16" s="109">
         <f>Assumptions!$B$12</f>
@@ -6339,7 +6541,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B17" s="112">
         <f>Assumptions!$B$13</f>
@@ -6348,7 +6550,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B18" s="109">
         <f>B16*B17</f>
@@ -6357,7 +6559,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B19" s="109">
         <f>IF(ISBLANK('Base Case'!G20),'Base Case'!F20,'Base Case'!G20)</f>
@@ -6366,7 +6568,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B20" s="109">
         <f>IF(ISBLANK('Base Case'!G25),'Base Case'!F25,'Base Case'!G25)</f>
@@ -6375,7 +6577,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="22" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B22" s="6">
         <f>IF(ISERROR(B7*(B18/(B20+B18))+B12*(B20/(B18+B20))*(1-B13)),0,B7*(B18/(B20+B18))+B12*(B20/(B18+B20))*(1-B13))</f>
@@ -6413,12 +6615,12 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="22" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="3" s="21" spans="1:16" thickBot="1">
       <c r="A3" s="25" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B3" s="58">
         <f>'Base Case'!B3</f>
@@ -6465,19 +6667,19 @@
         <v/>
       </c>
       <c r="M3" s="23" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="N3" s="26" t="n"/>
       <c r="O3" s="58" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P3" s="23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="27" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B4" s="101">
         <f>'Base Case'!B$8</f>
@@ -6526,7 +6728,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="27" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B5" s="101">
         <f>-'Base Case'!B$10</f>
@@ -6575,7 +6777,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="27" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B6" s="101">
         <f>'Base Case'!B$16</f>
@@ -6624,7 +6826,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="27" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B7" s="101">
         <f>'Base Case'!B$30</f>
@@ -6673,7 +6875,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="8" s="21" spans="1:16" thickBot="1">
       <c r="A8" s="34" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B8" s="113">
         <f>-'Base Case'!B$15</f>
@@ -6726,7 +6928,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="17" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B9" s="101">
         <f>SUM(B$4:B$8)</f>
@@ -6787,7 +6989,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="31" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B10" s="116" t="n"/>
       <c r="C10" s="116" t="n"/>
@@ -6831,7 +7033,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="12" s="21" spans="1:16" thickBot="1">
       <c r="A12" s="25" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B12" s="58">
         <f>B3</f>
@@ -6878,19 +7080,19 @@
         <v/>
       </c>
       <c r="M12" s="23" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="N12" s="26" t="n"/>
       <c r="O12" s="58" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P12" s="23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="27" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B13" s="101">
         <f>'Base Case'!B$8</f>
@@ -6940,7 +7142,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="27" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B14" s="101">
         <f>-'Base Case'!B$10</f>
@@ -6990,7 +7192,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="27" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B15" s="101">
         <f>'Base Case'!B$16</f>
@@ -7040,7 +7242,7 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="27" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B16" s="101">
         <f>'Base Case'!B$30</f>
@@ -7090,7 +7292,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="17" s="21" spans="1:16" thickBot="1">
       <c r="A17" s="34" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B17" s="113">
         <f>-'Base Case'!B$15</f>
@@ -7143,7 +7345,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="17" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B18" s="101">
         <f>SUM(B$4:B$8)</f>
@@ -7204,7 +7406,7 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="31" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B19" s="22" t="n"/>
       <c r="C19" s="22" t="n"/>
@@ -7248,7 +7450,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="21" s="21" spans="1:16" thickBot="1">
       <c r="A21" s="25" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B21" s="58">
         <f>B3</f>
@@ -7295,19 +7497,19 @@
         <v/>
       </c>
       <c r="M21" s="23" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="N21" s="26" t="n"/>
       <c r="O21" s="58" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P21" s="23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="27" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B22" s="101">
         <f>'Base Case'!B$8</f>
@@ -7360,7 +7562,7 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="27" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B23" s="101">
         <f>-'Base Case'!B$10</f>
@@ -7413,7 +7615,7 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="27" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B24" s="101">
         <f>'Base Case'!B$16</f>
@@ -7466,7 +7668,7 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="27" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B25" s="101">
         <f>'Base Case'!B$30</f>
@@ -7519,7 +7721,7 @@
     </row>
     <row customHeight="1" ht="15.75" r="26" s="21" spans="1:16" thickBot="1">
       <c r="A26" s="34" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B26" s="113">
         <f>-'Base Case'!B$15</f>
@@ -7572,7 +7774,7 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="17" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B27" s="101">
         <f>SUM(B$4:B$8)</f>
@@ -7634,7 +7836,7 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="31" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B28" s="22" t="n"/>
       <c r="C28" s="22" t="n"/>
@@ -7707,29 +7909,29 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="22" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="3" s="21" spans="1:9" thickBot="1">
       <c r="A3" s="25" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C3" s="26" t="n"/>
       <c r="D3" s="58" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E3" s="26" t="n"/>
       <c r="F3" s="58" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H3" s="22" t="n"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="27" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B4" s="119">
         <f>Assumptions!$F$16</f>
@@ -7749,7 +7951,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="27" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B5" s="119">
         <f>'Cash Flow Calculations'!$P$10</f>
@@ -7778,7 +7980,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="27" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B7" s="119">
         <f>'WACC Calculations'!$B$20</f>
@@ -7798,7 +8000,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="27" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B8" s="119">
         <f>'WACC Calculations'!$B$19</f>
@@ -7818,7 +8020,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="27" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B9" s="119">
         <f>B5-B7+B8</f>
@@ -7846,7 +8048,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="68" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B11" s="121">
         <f>B9/B4</f>
@@ -7865,7 +8067,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="76" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B12" s="74">
         <f>B11/Assumptions!$B$13-1</f>
@@ -7885,7 +8087,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="76" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B13" s="90" t="n"/>
       <c r="C13" s="72" t="n"/>
@@ -7905,7 +8107,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="68" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B15" s="122">
         <f>(B13*B11)+(D13*D11)+(F13*F11)</f>
@@ -7914,7 +8116,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="76" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B16" s="6">
         <f>B15/Assumptions!$B$13-1</f>

</xml_diff>